<commit_message>
Major data changes and revised data review due to updated response coding in access database
</commit_message>
<xml_diff>
--- a/Data Type.xlsx
+++ b/Data Type.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="Data_Type"/>
   </sheets>
   <definedNames>
-    <definedName name="Data_Type">'Data_Type'!$A$1:$C$18</definedName>
+    <definedName name="Data_Type">'Data_Type'!$A$1:$C$14</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -409,7 +409,7 @@
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>Current velocity, residnece times and related measures</t>
+          <t>Current velocity, residence times and related measures</t>
         </is>
       </c>
     </row>
@@ -424,32 +424,32 @@
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>Dissolved oxygen, chlorophyll, nutrients, clarity, etc.</t>
+          <t>Dissolved oxygen, chlorophyll, nutrients, clarity, or multiple metrics</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="6">
       <c r="A6" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>Habitat Analysis</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>Analysis of water as habitat or to provide insight into where conditions are suitable for certain species</t>
+          <t>Self explanatory</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="7">
       <c r="A7" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>Temperature</t>
+          <t>Salinity</t>
         </is>
       </c>
       <c r="C7" s="0" t="inlineStr">
@@ -460,168 +460,124 @@
     </row>
     <row outlineLevel="0" r="8">
       <c r="A8" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>Salinity</t>
+          <t>Inundation</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>Self explanatory</t>
+          <t>Areas that are or will be inundated.  May include depth or other details</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="9">
       <c r="A9" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Inundation</t>
+          <t>Erosion</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
         <is>
-          <t>Areas that are or will be inundated.  May include depth or other details</t>
+          <t>Rate or risk of shoreline erosion</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="10">
       <c r="A10" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>Erosion</t>
+          <t>Sediment</t>
         </is>
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
-          <t>Models that inform shoreline erosion, of multiple shoreline types</t>
+          <t>Sediment deposition,  erosion or transport in shallow waters</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="11">
       <c r="A11" s="0">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>Sediment</t>
+          <t>Transport</t>
         </is>
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>Data on sediment deposition,  erosion or transport in shallow waters.</t>
+          <t>Movement of pollutants, plankton, fish larvae, drifting objects, etc.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="12">
       <c r="A12" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>Transport</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="C12" s="0" t="inlineStr">
         <is>
-          <t>Data on movement of pollutants, plankton, fish larvae, drifting objects, etc.</t>
+          <t>Something that does not fit into other categories</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="13">
       <c r="A13" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>Other</t>
-        </is>
-      </c>
-      <c r="C13" s="0" t="inlineStr">
-        <is>
-          <t>Something that does not fit into other categories</t>
-        </is>
-      </c>
+          <t>Not Specified</t>
+        </is>
+      </c>
+      <c r="C13" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="14">
       <c r="A14" s="0">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>Freshwater</t>
         </is>
       </c>
       <c r="C14" s="0" t="inlineStr">
         <is>
-          <t>No clear category of data specified</t>
+          <t>Data on freshwater inflows, etc.</t>
         </is>
       </c>
     </row>
     <row outlineLevel="0" r="15">
-      <c r="A15" s="0">
-        <v>15</v>
-      </c>
-      <c r="B15" s="0" t="inlineStr">
-        <is>
-          <t>Ice</t>
-        </is>
-      </c>
-      <c r="C15" s="0" t="inlineStr">
-        <is>
-          <t>Ice data</t>
-        </is>
-      </c>
+      <c r="A15" s="0"/>
+      <c r="B15" s="0" t="inlineStr"/>
+      <c r="C15" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="16">
-      <c r="A16" s="0">
-        <v>16</v>
-      </c>
-      <c r="B16" s="0" t="inlineStr">
-        <is>
-          <t>Freshwater</t>
-        </is>
-      </c>
-      <c r="C16" s="0" t="inlineStr">
-        <is>
-          <t>Data on freshwater inflows, etc.</t>
-        </is>
-      </c>
+      <c r="A16" s="0"/>
+      <c r="B16" s="0" t="inlineStr"/>
+      <c r="C16" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="17">
-      <c r="A17" s="0">
-        <v>17</v>
-      </c>
-      <c r="B17" s="0" t="inlineStr">
-        <is>
-          <t>Weather</t>
-        </is>
-      </c>
-      <c r="C17" s="0" t="inlineStr">
-        <is>
-          <t>Atmospheric conditions</t>
-        </is>
-      </c>
+      <c r="A17" s="0"/>
+      <c r="B17" s="0" t="inlineStr"/>
+      <c r="C17" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="18">
-      <c r="A18" s="0">
-        <v>18</v>
-      </c>
-      <c r="B18" s="0" t="inlineStr">
-        <is>
-          <t>Biological</t>
-        </is>
-      </c>
-      <c r="C18" s="0" t="inlineStr">
-        <is>
-          <t>Data on marine ecosystems or biota</t>
-        </is>
-      </c>
+      <c r="A18" s="0"/>
+      <c r="B18" s="0" t="inlineStr"/>
+      <c r="C18" s="0" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>